<commit_message>
fixed ages in levine
</commit_message>
<xml_diff>
--- a/dna-methylation/routines/levine/levine.xlsx
+++ b/dna-methylation/routines/levine/levine.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\dna-methylation\dna-methylation\routines\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\dna-methylation\dna-methylation\routines\levine\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -209,8 +209,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="d\.m"/>
-    <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="d\.m"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -367,12 +367,12 @@
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -433,7 +433,7 @@
     <xf numFmtId="2" fontId="1" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -442,7 +442,7 @@
     <xf numFmtId="1" fontId="1" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -731,7 +731,7 @@
   <dimension ref="A1:AG45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H43" sqref="H43"/>
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2614,7 +2614,7 @@
         <v>45</v>
       </c>
       <c r="B36" s="9">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="C36" s="9">
         <v>40.4</v>

</xml_diff>

<commit_message>
levine plot for report
</commit_message>
<xml_diff>
--- a/dna-methylation/routines/levine/levine.xlsx
+++ b/dna-methylation/routines/levine/levine.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="62">
   <si>
     <t>Name</t>
   </si>
@@ -202,6 +202,9 @@
   </si>
   <si>
     <t>01_10</t>
+  </si>
+  <si>
+    <t>PA</t>
   </si>
 </sst>
 </file>
@@ -728,65 +731,68 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AG45"/>
+  <dimension ref="A1:AH45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+      <selection activeCell="B40" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24" style="3"/>
-    <col min="2" max="3" width="24" style="9"/>
-    <col min="4" max="16384" width="24" style="3"/>
+    <col min="2" max="4" width="24" style="9"/>
+    <col min="5" max="16384" width="24" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="AA1" s="1"/>
       <c r="AB1" s="1"/>
       <c r="AC1" s="1"/>
       <c r="AD1" s="1"/>
       <c r="AE1" s="1"/>
-      <c r="AF1" s="4"/>
+      <c r="AF1" s="1"/>
       <c r="AG1" s="4"/>
-    </row>
-    <row r="2" spans="1:33" s="25" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AH1" s="4"/>
+    </row>
+    <row r="2" spans="1:34" s="25" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
         <v>24</v>
       </c>
@@ -794,55 +800,58 @@
         <v>92</v>
       </c>
       <c r="C2" s="27">
+        <v>94.75</v>
+      </c>
+      <c r="D2" s="27">
         <v>44.4</v>
       </c>
-      <c r="D2" s="28">
+      <c r="E2" s="28">
         <v>50.9</v>
       </c>
-      <c r="E2" s="29">
+      <c r="F2" s="29">
         <v>7.26</v>
       </c>
-      <c r="F2" s="29">
+      <c r="G2" s="29">
         <v>262.89999999999998</v>
       </c>
-      <c r="G2" s="28">
+      <c r="H2" s="28">
         <v>36</v>
       </c>
-      <c r="H2" s="30">
+      <c r="I2" s="30">
         <v>91</v>
       </c>
-      <c r="I2" s="28">
+      <c r="J2" s="28">
         <v>15</v>
       </c>
-      <c r="J2" s="28">
+      <c r="K2" s="28">
         <v>164.9</v>
       </c>
-      <c r="K2" s="27">
+      <c r="L2" s="27">
         <v>3.47</v>
       </c>
-      <c r="L2" s="29"/>
       <c r="M2" s="29"/>
-      <c r="N2" s="31"/>
-      <c r="O2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="31"/>
       <c r="P2" s="29"/>
       <c r="Q2" s="29"/>
-      <c r="R2" s="31"/>
-      <c r="S2" s="29"/>
+      <c r="R2" s="29"/>
+      <c r="S2" s="31"/>
       <c r="T2" s="29"/>
       <c r="U2" s="29"/>
-      <c r="V2" s="31"/>
-      <c r="W2" s="29"/>
+      <c r="V2" s="29"/>
+      <c r="W2" s="31"/>
       <c r="X2" s="29"/>
       <c r="Y2" s="29"/>
       <c r="Z2" s="29"/>
-      <c r="AA2" s="31"/>
-      <c r="AB2" s="29"/>
+      <c r="AA2" s="29"/>
+      <c r="AB2" s="31"/>
       <c r="AC2" s="29"/>
       <c r="AD2" s="29"/>
       <c r="AE2" s="29"/>
       <c r="AF2" s="29"/>
-    </row>
-    <row r="3" spans="1:33" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AG2" s="29"/>
+    </row>
+    <row r="3" spans="1:34" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>25</v>
       </c>
@@ -850,57 +859,60 @@
         <v>90</v>
       </c>
       <c r="C3" s="8">
+        <v>85.84</v>
+      </c>
+      <c r="D3" s="8">
         <v>46.5</v>
       </c>
-      <c r="D3" s="6">
+      <c r="E3" s="6">
         <v>24.9</v>
       </c>
-      <c r="E3" s="1">
+      <c r="F3" s="1">
         <v>6.06</v>
       </c>
-      <c r="F3" s="1">
+      <c r="G3" s="1">
         <v>229.1</v>
       </c>
-      <c r="G3" s="6">
+      <c r="H3" s="6">
         <v>21</v>
       </c>
-      <c r="H3" s="5">
+      <c r="I3" s="5">
         <v>90</v>
       </c>
-      <c r="I3" s="6">
+      <c r="J3" s="6">
         <v>14.1</v>
       </c>
-      <c r="J3" s="6">
+      <c r="K3" s="6">
         <v>149.5</v>
       </c>
-      <c r="K3" s="8">
+      <c r="L3" s="8">
         <v>5.07</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="M3" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="M3" s="1"/>
-      <c r="N3" s="7"/>
-      <c r="O3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="7"/>
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
-      <c r="R3" s="7"/>
-      <c r="S3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="7"/>
       <c r="T3" s="1"/>
       <c r="U3" s="1"/>
-      <c r="V3" s="7"/>
-      <c r="W3" s="1"/>
+      <c r="V3" s="1"/>
+      <c r="W3" s="7"/>
       <c r="X3" s="1"/>
       <c r="Y3" s="1"/>
       <c r="Z3" s="1"/>
-      <c r="AA3" s="7"/>
-      <c r="AB3" s="1"/>
+      <c r="AA3" s="1"/>
+      <c r="AB3" s="7"/>
       <c r="AC3" s="1"/>
       <c r="AD3" s="1"/>
       <c r="AE3" s="1"/>
       <c r="AF3" s="1"/>
-    </row>
-    <row r="4" spans="1:33" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AG3" s="1"/>
+    </row>
+    <row r="4" spans="1:34" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>26</v>
       </c>
@@ -908,57 +920,60 @@
         <v>61</v>
       </c>
       <c r="C4" s="8">
+        <v>65.09</v>
+      </c>
+      <c r="D4" s="8">
         <v>40.799999999999997</v>
       </c>
-      <c r="D4" s="6">
+      <c r="E4" s="6">
         <v>52.1</v>
       </c>
-      <c r="E4" s="1">
+      <c r="F4" s="1">
         <v>6.39</v>
       </c>
-      <c r="F4" s="1">
+      <c r="G4" s="1">
         <v>149.6</v>
       </c>
-      <c r="G4" s="6">
+      <c r="H4" s="6">
         <v>23.5</v>
       </c>
-      <c r="H4" s="5">
+      <c r="I4" s="5">
         <v>92</v>
       </c>
-      <c r="I4" s="6">
+      <c r="J4" s="6">
         <v>14.3</v>
       </c>
-      <c r="J4" s="6">
+      <c r="K4" s="6">
         <v>141.69999999999999</v>
       </c>
-      <c r="K4" s="8">
+      <c r="L4" s="8">
         <v>3.07</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="M4" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="M4" s="1"/>
-      <c r="N4" s="7"/>
-      <c r="O4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="7"/>
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
-      <c r="R4" s="7"/>
-      <c r="S4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="7"/>
       <c r="T4" s="1"/>
       <c r="U4" s="1"/>
-      <c r="V4" s="7"/>
-      <c r="W4" s="1"/>
+      <c r="V4" s="1"/>
+      <c r="W4" s="7"/>
       <c r="X4" s="1"/>
       <c r="Y4" s="1"/>
       <c r="Z4" s="1"/>
-      <c r="AA4" s="7"/>
-      <c r="AB4" s="1"/>
+      <c r="AA4" s="1"/>
+      <c r="AB4" s="7"/>
       <c r="AC4" s="1"/>
       <c r="AD4" s="1"/>
       <c r="AE4" s="1"/>
       <c r="AF4" s="1"/>
-    </row>
-    <row r="5" spans="1:33" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AG4" s="1"/>
+    </row>
+    <row r="5" spans="1:34" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>27</v>
       </c>
@@ -966,57 +981,60 @@
         <v>28</v>
       </c>
       <c r="C5" s="8">
+        <v>34.72</v>
+      </c>
+      <c r="D5" s="8">
         <v>42.6</v>
       </c>
-      <c r="D5" s="6">
+      <c r="E5" s="6">
         <v>88.5</v>
       </c>
-      <c r="E5" s="1">
+      <c r="F5" s="1">
         <v>5.68</v>
       </c>
-      <c r="F5" s="1">
+      <c r="G5" s="1">
         <v>104.4</v>
       </c>
-      <c r="G5" s="6">
+      <c r="H5" s="6">
         <v>40.799999999999997</v>
       </c>
-      <c r="H5" s="5">
+      <c r="I5" s="5">
         <v>85</v>
       </c>
-      <c r="I5" s="6">
+      <c r="J5" s="6">
         <v>15</v>
       </c>
-      <c r="J5" s="6">
+      <c r="K5" s="6">
         <v>103.9</v>
       </c>
-      <c r="K5" s="8">
+      <c r="L5" s="8">
         <v>3.4</v>
       </c>
-      <c r="L5" s="1" t="s">
+      <c r="M5" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="M5" s="1"/>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
-      <c r="R5" s="7"/>
-      <c r="S5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="7"/>
       <c r="T5" s="1"/>
       <c r="U5" s="1"/>
-      <c r="V5" s="7"/>
-      <c r="W5" s="1"/>
+      <c r="V5" s="1"/>
+      <c r="W5" s="7"/>
       <c r="X5" s="1"/>
       <c r="Y5" s="1"/>
       <c r="Z5" s="1"/>
-      <c r="AA5" s="7"/>
-      <c r="AB5" s="1"/>
+      <c r="AA5" s="1"/>
+      <c r="AB5" s="7"/>
       <c r="AC5" s="1"/>
       <c r="AD5" s="1"/>
       <c r="AE5" s="1"/>
       <c r="AF5" s="1"/>
-    </row>
-    <row r="6" spans="1:33" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AG5" s="1"/>
+    </row>
+    <row r="6" spans="1:34" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>28</v>
       </c>
@@ -1024,57 +1042,60 @@
         <v>32</v>
       </c>
       <c r="C6" s="8">
+        <v>31.07</v>
+      </c>
+      <c r="D6" s="8">
         <v>46</v>
       </c>
-      <c r="D6" s="6">
+      <c r="E6" s="6">
         <v>59.2</v>
       </c>
-      <c r="E6" s="1">
+      <c r="F6" s="1">
         <v>5.18</v>
       </c>
-      <c r="F6" s="1">
+      <c r="G6" s="1">
         <v>134.5</v>
       </c>
-      <c r="G6" s="6">
+      <c r="H6" s="6">
         <v>41.9</v>
       </c>
-      <c r="H6" s="5">
+      <c r="I6" s="5">
         <v>84</v>
       </c>
-      <c r="I6" s="6">
+      <c r="J6" s="6">
         <v>14.4</v>
       </c>
-      <c r="J6" s="6">
+      <c r="K6" s="6">
         <v>100.1</v>
       </c>
-      <c r="K6" s="8">
+      <c r="L6" s="8">
         <v>4.76</v>
       </c>
-      <c r="L6" s="1" t="s">
+      <c r="M6" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="M6" s="1"/>
-      <c r="N6" s="7"/>
-      <c r="O6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="7"/>
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
-      <c r="R6" s="7"/>
-      <c r="S6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="7"/>
       <c r="T6" s="1"/>
       <c r="U6" s="1"/>
-      <c r="V6" s="7"/>
-      <c r="W6" s="1"/>
+      <c r="V6" s="1"/>
+      <c r="W6" s="7"/>
       <c r="X6" s="1"/>
       <c r="Y6" s="1"/>
       <c r="Z6" s="1"/>
-      <c r="AA6" s="7"/>
-      <c r="AB6" s="1"/>
+      <c r="AA6" s="1"/>
+      <c r="AB6" s="7"/>
       <c r="AC6" s="1"/>
       <c r="AD6" s="1"/>
       <c r="AE6" s="1"/>
       <c r="AF6" s="1"/>
-    </row>
-    <row r="7" spans="1:33" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AG6" s="1"/>
+    </row>
+    <row r="7" spans="1:34" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
         <v>29</v>
       </c>
@@ -1082,57 +1103,60 @@
         <v>68</v>
       </c>
       <c r="C7" s="8">
+        <v>71.05</v>
+      </c>
+      <c r="D7" s="8">
         <v>39.700000000000003</v>
       </c>
-      <c r="D7" s="6">
+      <c r="E7" s="6">
         <v>45.7</v>
       </c>
-      <c r="E7" s="1">
+      <c r="F7" s="1">
         <v>6.06</v>
       </c>
-      <c r="F7" s="1">
+      <c r="G7" s="1">
         <v>241.2</v>
       </c>
-      <c r="G7" s="6">
+      <c r="H7" s="6">
         <v>21</v>
       </c>
-      <c r="H7" s="5">
+      <c r="I7" s="5">
         <v>90</v>
       </c>
-      <c r="I7" s="6">
+      <c r="J7" s="6">
         <v>14.6</v>
       </c>
-      <c r="J7" s="6">
+      <c r="K7" s="6">
         <v>77.599999999999994</v>
       </c>
-      <c r="K7" s="8">
+      <c r="L7" s="8">
         <v>4.68</v>
       </c>
-      <c r="L7" s="1" t="s">
+      <c r="M7" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="M7" s="1"/>
-      <c r="N7" s="7"/>
-      <c r="O7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="7"/>
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
-      <c r="R7" s="7"/>
-      <c r="S7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="7"/>
       <c r="T7" s="1"/>
       <c r="U7" s="1"/>
-      <c r="V7" s="7"/>
-      <c r="W7" s="1"/>
+      <c r="V7" s="1"/>
+      <c r="W7" s="7"/>
       <c r="X7" s="1"/>
       <c r="Y7" s="1"/>
       <c r="Z7" s="1"/>
-      <c r="AA7" s="7"/>
-      <c r="AB7" s="1"/>
+      <c r="AA7" s="1"/>
+      <c r="AB7" s="7"/>
       <c r="AC7" s="1"/>
       <c r="AD7" s="1"/>
       <c r="AE7" s="1"/>
       <c r="AF7" s="1"/>
-    </row>
-    <row r="8" spans="1:33" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AG7" s="1"/>
+    </row>
+    <row r="8" spans="1:34" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
         <v>30</v>
       </c>
@@ -1140,57 +1164,60 @@
         <v>37</v>
       </c>
       <c r="C8" s="8">
+        <v>39.799999999999997</v>
+      </c>
+      <c r="D8" s="8">
         <v>52.2</v>
       </c>
-      <c r="D8" s="6">
+      <c r="E8" s="6">
         <v>45.2</v>
       </c>
-      <c r="E8" s="1">
+      <c r="F8" s="1">
         <v>4.82</v>
       </c>
-      <c r="F8" s="1">
+      <c r="G8" s="1">
         <v>112.1</v>
       </c>
-      <c r="G8" s="6">
+      <c r="H8" s="6">
         <v>18.5</v>
       </c>
-      <c r="H8" s="5">
+      <c r="I8" s="5">
         <v>83</v>
       </c>
-      <c r="I8" s="6">
+      <c r="J8" s="6">
         <v>15.4</v>
       </c>
-      <c r="J8" s="6">
+      <c r="K8" s="6">
         <v>226.2</v>
       </c>
-      <c r="K8" s="8">
+      <c r="L8" s="8">
         <v>4.4000000000000004</v>
       </c>
-      <c r="L8" s="1" t="s">
+      <c r="M8" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="M8" s="1"/>
-      <c r="N8" s="7"/>
-      <c r="O8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="7"/>
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
-      <c r="R8" s="7"/>
-      <c r="S8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="7"/>
       <c r="T8" s="1"/>
       <c r="U8" s="1"/>
-      <c r="V8" s="7"/>
-      <c r="W8" s="1"/>
+      <c r="V8" s="1"/>
+      <c r="W8" s="7"/>
       <c r="X8" s="1"/>
       <c r="Y8" s="1"/>
       <c r="Z8" s="1"/>
-      <c r="AA8" s="7"/>
-      <c r="AB8" s="1"/>
+      <c r="AA8" s="1"/>
+      <c r="AB8" s="7"/>
       <c r="AC8" s="1"/>
       <c r="AD8" s="1"/>
       <c r="AE8" s="1"/>
       <c r="AF8" s="1"/>
-    </row>
-    <row r="9" spans="1:33" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AG8" s="1"/>
+    </row>
+    <row r="9" spans="1:34" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>31</v>
       </c>
@@ -1198,36 +1225,38 @@
         <v>41</v>
       </c>
       <c r="C9" s="8">
+        <v>30.2</v>
+      </c>
+      <c r="D9" s="8">
         <v>58.5</v>
       </c>
-      <c r="D9" s="6">
+      <c r="E9" s="6">
         <v>73.900000000000006</v>
       </c>
-      <c r="E9" s="1">
+      <c r="F9" s="1">
         <v>3.53</v>
       </c>
-      <c r="F9" s="1">
+      <c r="G9" s="1">
         <v>256.2</v>
       </c>
-      <c r="G9" s="6">
+      <c r="H9" s="6">
         <v>41.5</v>
       </c>
-      <c r="H9" s="5">
+      <c r="I9" s="5">
         <v>91</v>
       </c>
-      <c r="I9" s="6">
+      <c r="J9" s="6">
         <v>13.1</v>
       </c>
-      <c r="J9" s="6">
+      <c r="K9" s="6">
         <v>118.6</v>
       </c>
-      <c r="K9" s="8">
+      <c r="L9" s="8">
         <v>4.33</v>
       </c>
-      <c r="L9" s="1" t="s">
+      <c r="M9" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="M9" s="1"/>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
@@ -1241,14 +1270,15 @@
       <c r="X9" s="1"/>
       <c r="Y9" s="1"/>
       <c r="Z9" s="1"/>
-      <c r="AA9" s="7"/>
-      <c r="AB9" s="1"/>
+      <c r="AA9" s="1"/>
+      <c r="AB9" s="7"/>
       <c r="AC9" s="1"/>
       <c r="AD9" s="1"/>
       <c r="AE9" s="1"/>
       <c r="AF9" s="1"/>
-    </row>
-    <row r="10" spans="1:33" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AG9" s="1"/>
+    </row>
+    <row r="10" spans="1:34" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
         <v>32</v>
       </c>
@@ -1256,36 +1286,38 @@
         <v>15</v>
       </c>
       <c r="C10" s="8">
+        <v>17.54</v>
+      </c>
+      <c r="D10" s="8">
         <v>42.9</v>
       </c>
-      <c r="D10" s="6">
+      <c r="E10" s="6">
         <v>59.4</v>
       </c>
-      <c r="E10" s="1">
+      <c r="F10" s="1">
         <v>4.83</v>
       </c>
-      <c r="F10" s="1">
+      <c r="G10" s="1">
         <v>330.3</v>
       </c>
-      <c r="G10" s="6">
+      <c r="H10" s="6">
         <v>33.299999999999997</v>
       </c>
-      <c r="H10" s="5">
+      <c r="I10" s="5">
         <v>89</v>
       </c>
-      <c r="I10" s="6">
+      <c r="J10" s="6">
         <v>13.3</v>
       </c>
-      <c r="J10" s="6">
+      <c r="K10" s="6">
         <v>177.1</v>
       </c>
-      <c r="K10" s="8">
+      <c r="L10" s="8">
         <v>5.69</v>
       </c>
-      <c r="L10" s="1" t="s">
+      <c r="M10" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="M10" s="1"/>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
@@ -1299,14 +1331,15 @@
       <c r="X10" s="1"/>
       <c r="Y10" s="1"/>
       <c r="Z10" s="1"/>
-      <c r="AA10" s="7"/>
-      <c r="AB10" s="1"/>
+      <c r="AA10" s="1"/>
+      <c r="AB10" s="7"/>
       <c r="AC10" s="1"/>
       <c r="AD10" s="1"/>
       <c r="AE10" s="1"/>
       <c r="AF10" s="1"/>
-    </row>
-    <row r="11" spans="1:33" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AG10" s="1"/>
+    </row>
+    <row r="11" spans="1:34" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
         <v>33</v>
       </c>
@@ -1314,36 +1347,38 @@
         <v>91</v>
       </c>
       <c r="C11" s="8">
+        <v>79.81</v>
+      </c>
+      <c r="D11" s="8">
         <v>40.9</v>
       </c>
-      <c r="D11" s="6">
+      <c r="E11" s="6">
         <v>87.1</v>
       </c>
-      <c r="E11" s="1">
+      <c r="F11" s="1">
         <v>2.44</v>
       </c>
-      <c r="F11" s="1">
+      <c r="G11" s="1">
         <v>133.19999999999999</v>
       </c>
-      <c r="G11" s="6">
+      <c r="H11" s="6">
         <v>47.5</v>
       </c>
-      <c r="H11" s="5">
+      <c r="I11" s="5">
         <v>93</v>
       </c>
-      <c r="I11" s="6">
+      <c r="J11" s="6">
         <v>13.1</v>
       </c>
-      <c r="J11" s="6">
+      <c r="K11" s="6">
         <v>79.2</v>
       </c>
-      <c r="K11" s="8">
+      <c r="L11" s="8">
         <v>5.57</v>
       </c>
-      <c r="L11" s="1" t="s">
+      <c r="M11" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="M11" s="1"/>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
@@ -1355,15 +1390,16 @@
       <c r="V11" s="1"/>
       <c r="W11" s="1"/>
       <c r="X11" s="1"/>
-      <c r="Z11" s="1"/>
+      <c r="Y11" s="1"/>
       <c r="AA11" s="1"/>
       <c r="AB11" s="1"/>
       <c r="AC11" s="1"/>
       <c r="AD11" s="1"/>
       <c r="AE11" s="1"/>
       <c r="AF11" s="1"/>
-    </row>
-    <row r="12" spans="1:33" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AG11" s="1"/>
+    </row>
+    <row r="12" spans="1:34" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="19" t="s">
         <v>34</v>
       </c>
@@ -1371,36 +1407,38 @@
         <v>65</v>
       </c>
       <c r="C12" s="8">
+        <v>64.28</v>
+      </c>
+      <c r="D12" s="8">
         <v>38.9</v>
       </c>
-      <c r="D12" s="6">
+      <c r="E12" s="6">
         <v>93.9</v>
       </c>
-      <c r="E12" s="1">
+      <c r="F12" s="1">
         <v>3.21</v>
       </c>
-      <c r="F12" s="1">
+      <c r="G12" s="1">
         <v>171.1</v>
       </c>
-      <c r="G12" s="6">
+      <c r="H12" s="6">
         <v>50.8</v>
       </c>
-      <c r="H12" s="5">
+      <c r="I12" s="5">
         <v>98</v>
       </c>
-      <c r="I12" s="6">
+      <c r="J12" s="6">
         <v>13.3</v>
       </c>
-      <c r="J12" s="6">
+      <c r="K12" s="6">
         <v>219.4</v>
       </c>
-      <c r="K12" s="8">
+      <c r="L12" s="8">
         <v>5.05</v>
       </c>
-      <c r="L12" s="1" t="s">
+      <c r="M12" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="M12" s="1"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
@@ -1412,15 +1450,16 @@
       <c r="V12" s="1"/>
       <c r="W12" s="1"/>
       <c r="X12" s="1"/>
-      <c r="Z12" s="1"/>
+      <c r="Y12" s="1"/>
       <c r="AA12" s="1"/>
       <c r="AB12" s="1"/>
       <c r="AC12" s="1"/>
       <c r="AD12" s="1"/>
       <c r="AE12" s="1"/>
       <c r="AF12" s="1"/>
-    </row>
-    <row r="13" spans="1:33" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AG12" s="1"/>
+    </row>
+    <row r="13" spans="1:34" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
         <v>35</v>
       </c>
@@ -1428,36 +1467,38 @@
         <v>43</v>
       </c>
       <c r="C13" s="8">
+        <v>59.04</v>
+      </c>
+      <c r="D13" s="8">
         <v>24.8</v>
       </c>
-      <c r="D13" s="6">
+      <c r="E13" s="6">
         <v>107.5</v>
       </c>
-      <c r="E13" s="1">
+      <c r="F13" s="1">
         <v>5.33</v>
       </c>
-      <c r="F13" s="1">
+      <c r="G13" s="1">
         <v>518.1</v>
       </c>
-      <c r="G13" s="6">
+      <c r="H13" s="6">
         <v>21.7</v>
       </c>
-      <c r="H13" s="5">
+      <c r="I13" s="5">
         <v>90</v>
       </c>
-      <c r="I13" s="6">
+      <c r="J13" s="6">
         <v>13.5</v>
       </c>
-      <c r="J13" s="6">
+      <c r="K13" s="6">
         <v>118.3</v>
       </c>
-      <c r="K13" s="8">
+      <c r="L13" s="8">
         <v>9.1</v>
       </c>
-      <c r="L13" s="1" t="s">
+      <c r="M13" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="M13" s="1"/>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
@@ -1469,15 +1510,16 @@
       <c r="V13" s="1"/>
       <c r="W13" s="1"/>
       <c r="X13" s="1"/>
-      <c r="Z13" s="1"/>
+      <c r="Y13" s="1"/>
       <c r="AA13" s="1"/>
       <c r="AB13" s="1"/>
       <c r="AC13" s="1"/>
       <c r="AD13" s="1"/>
       <c r="AE13" s="1"/>
       <c r="AF13" s="1"/>
-    </row>
-    <row r="14" spans="1:33" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AG13" s="1"/>
+    </row>
+    <row r="14" spans="1:34" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="20" t="s">
         <v>36</v>
       </c>
@@ -1485,36 +1527,38 @@
         <v>88</v>
       </c>
       <c r="C14" s="8">
+        <v>80.41</v>
+      </c>
+      <c r="D14" s="8">
         <v>48.1</v>
       </c>
-      <c r="D14" s="6">
+      <c r="E14" s="6">
         <v>53.2</v>
       </c>
-      <c r="E14" s="1">
+      <c r="F14" s="1">
         <v>6.06</v>
       </c>
-      <c r="F14" s="1">
+      <c r="G14" s="1">
         <v>70.8</v>
       </c>
-      <c r="G14" s="6">
+      <c r="H14" s="6">
         <v>54.1</v>
       </c>
-      <c r="H14" s="5">
+      <c r="I14" s="5">
         <v>86</v>
       </c>
-      <c r="I14" s="6">
+      <c r="J14" s="6">
         <v>13.8</v>
       </c>
-      <c r="J14" s="6">
+      <c r="K14" s="6">
         <v>165.8</v>
       </c>
-      <c r="K14" s="8">
+      <c r="L14" s="8">
         <v>6.47</v>
       </c>
-      <c r="L14" s="1" t="s">
+      <c r="M14" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="M14" s="1"/>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
@@ -1534,8 +1578,9 @@
       <c r="AD14" s="1"/>
       <c r="AE14" s="1"/>
       <c r="AF14" s="1"/>
-    </row>
-    <row r="15" spans="1:33" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AG14" s="1"/>
+    </row>
+    <row r="15" spans="1:34" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="20" t="s">
         <v>37</v>
       </c>
@@ -1543,36 +1588,38 @@
         <v>57</v>
       </c>
       <c r="C15" s="8">
+        <v>53.72</v>
+      </c>
+      <c r="D15" s="8">
         <v>56.7</v>
       </c>
-      <c r="D15" s="6">
+      <c r="E15" s="6">
         <v>64.5</v>
       </c>
-      <c r="E15" s="1">
+      <c r="F15" s="1">
         <v>7.83</v>
       </c>
-      <c r="F15" s="1">
+      <c r="G15" s="1">
         <v>125.3</v>
       </c>
-      <c r="G15" s="6">
+      <c r="H15" s="6">
         <v>78.5</v>
       </c>
-      <c r="H15" s="5">
+      <c r="I15" s="5">
         <v>87</v>
       </c>
-      <c r="I15" s="6">
+      <c r="J15" s="6">
         <v>13.8</v>
       </c>
-      <c r="J15" s="6">
+      <c r="K15" s="6">
         <v>198</v>
       </c>
-      <c r="K15" s="8">
+      <c r="L15" s="8">
         <v>8.33</v>
       </c>
-      <c r="L15" s="1" t="s">
+      <c r="M15" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="M15" s="1"/>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
@@ -1592,8 +1639,9 @@
       <c r="AD15" s="1"/>
       <c r="AE15" s="1"/>
       <c r="AF15" s="1"/>
-    </row>
-    <row r="16" spans="1:33" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AG15" s="1"/>
+    </row>
+    <row r="16" spans="1:34" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="21" t="s">
         <v>38</v>
       </c>
@@ -1601,36 +1649,38 @@
         <v>87</v>
       </c>
       <c r="C16" s="8">
+        <v>90.55</v>
+      </c>
+      <c r="D16" s="8">
         <v>42.1</v>
       </c>
-      <c r="D16" s="6">
+      <c r="E16" s="6">
         <v>71.8</v>
       </c>
-      <c r="E16" s="1">
+      <c r="F16" s="1">
         <v>6.71</v>
       </c>
-      <c r="F16" s="1">
+      <c r="G16" s="1">
         <v>362.5</v>
       </c>
-      <c r="G16" s="6">
+      <c r="H16" s="6">
         <v>51.2</v>
       </c>
-      <c r="H16" s="5">
+      <c r="I16" s="5">
         <v>90</v>
       </c>
-      <c r="I16" s="6">
+      <c r="J16" s="6">
         <v>15.6</v>
       </c>
-      <c r="J16" s="6">
+      <c r="K16" s="6">
         <v>123.9</v>
       </c>
-      <c r="K16" s="8">
+      <c r="L16" s="8">
         <v>2.2200000000000002</v>
       </c>
-      <c r="L16" s="1" t="s">
+      <c r="M16" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="M16" s="1"/>
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
@@ -1650,8 +1700,9 @@
       <c r="AD16" s="1"/>
       <c r="AE16" s="1"/>
       <c r="AF16" s="1"/>
-    </row>
-    <row r="17" spans="1:32" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AG16" s="1"/>
+    </row>
+    <row r="17" spans="1:33" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="21" t="s">
         <v>39</v>
       </c>
@@ -1659,36 +1710,38 @@
         <v>63</v>
       </c>
       <c r="C17" s="8">
+        <v>60.27</v>
+      </c>
+      <c r="D17" s="8">
         <v>57.9</v>
       </c>
-      <c r="D17" s="6">
+      <c r="E17" s="6">
         <v>77.599999999999994</v>
       </c>
-      <c r="E17" s="1">
+      <c r="F17" s="1">
         <v>6.77</v>
       </c>
-      <c r="F17" s="1">
+      <c r="G17" s="1">
         <v>146.69999999999999</v>
       </c>
-      <c r="G17" s="6">
+      <c r="H17" s="6">
         <v>28.6</v>
       </c>
-      <c r="H17" s="5">
+      <c r="I17" s="5">
         <v>87</v>
       </c>
-      <c r="I17" s="6">
+      <c r="J17" s="6">
         <v>13.6</v>
       </c>
-      <c r="J17" s="6">
+      <c r="K17" s="6">
         <v>208.3</v>
       </c>
-      <c r="K17" s="8">
+      <c r="L17" s="8">
         <v>2.41</v>
       </c>
-      <c r="L17" s="1" t="s">
+      <c r="M17" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="M17" s="1"/>
       <c r="N17" s="1"/>
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
@@ -1708,8 +1761,9 @@
       <c r="AD17" s="1"/>
       <c r="AE17" s="1"/>
       <c r="AF17" s="1"/>
-    </row>
-    <row r="18" spans="1:32" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AG17" s="1"/>
+    </row>
+    <row r="18" spans="1:33" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="21" t="s">
         <v>40</v>
       </c>
@@ -1717,36 +1771,38 @@
         <v>39</v>
       </c>
       <c r="C18" s="8">
+        <v>45.82</v>
+      </c>
+      <c r="D18" s="8">
         <v>53.9</v>
       </c>
-      <c r="D18" s="6">
+      <c r="E18" s="6">
         <v>113.7</v>
       </c>
-      <c r="E18" s="1">
+      <c r="F18" s="1">
         <v>5.67</v>
       </c>
-      <c r="F18" s="1">
+      <c r="G18" s="1">
         <v>148.6</v>
       </c>
-      <c r="G18" s="6">
+      <c r="H18" s="6">
         <v>36.4</v>
       </c>
-      <c r="H18" s="5">
+      <c r="I18" s="5">
         <v>97</v>
       </c>
-      <c r="I18" s="6">
+      <c r="J18" s="6">
         <v>13.8</v>
       </c>
-      <c r="J18" s="6">
+      <c r="K18" s="6">
         <v>187.1</v>
       </c>
-      <c r="K18" s="8">
+      <c r="L18" s="8">
         <v>5.36</v>
       </c>
-      <c r="L18" s="1" t="s">
+      <c r="M18" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="M18" s="1"/>
       <c r="N18" s="1"/>
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
@@ -1766,8 +1822,9 @@
       <c r="AD18" s="1"/>
       <c r="AE18" s="1"/>
       <c r="AF18" s="1"/>
-    </row>
-    <row r="19" spans="1:32" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AG18" s="1"/>
+    </row>
+    <row r="19" spans="1:33" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="22" t="s">
         <v>41</v>
       </c>
@@ -1775,36 +1832,38 @@
         <v>96</v>
       </c>
       <c r="C19" s="8">
+        <v>102.87</v>
+      </c>
+      <c r="D19" s="8">
         <v>23.8</v>
       </c>
-      <c r="D19" s="6">
+      <c r="E19" s="6">
         <v>99.2</v>
       </c>
-      <c r="E19" s="1">
+      <c r="F19" s="1">
         <v>5.95</v>
       </c>
-      <c r="F19" s="1">
+      <c r="G19" s="1">
         <v>100.7</v>
       </c>
-      <c r="G19" s="6">
+      <c r="H19" s="6">
         <v>35.799999999999997</v>
       </c>
-      <c r="H19" s="5">
+      <c r="I19" s="5">
         <v>87</v>
       </c>
-      <c r="I19" s="6">
+      <c r="J19" s="6">
         <v>14.1</v>
       </c>
-      <c r="J19" s="6">
+      <c r="K19" s="6">
         <v>106.2</v>
       </c>
-      <c r="K19" s="8">
+      <c r="L19" s="8">
         <v>4.72</v>
       </c>
-      <c r="L19" s="1" t="s">
+      <c r="M19" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="M19" s="1"/>
       <c r="N19" s="1"/>
       <c r="O19" s="1"/>
       <c r="P19" s="1"/>
@@ -1824,8 +1883,9 @@
       <c r="AD19" s="1"/>
       <c r="AE19" s="1"/>
       <c r="AF19" s="1"/>
-    </row>
-    <row r="20" spans="1:32" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AG19" s="1"/>
+    </row>
+    <row r="20" spans="1:33" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="22" t="s">
         <v>42</v>
       </c>
@@ -1833,36 +1893,38 @@
         <v>59</v>
       </c>
       <c r="C20" s="8">
+        <v>66.44</v>
+      </c>
+      <c r="D20" s="8">
         <v>46.8</v>
       </c>
-      <c r="D20" s="6">
+      <c r="E20" s="6">
         <v>95.2</v>
       </c>
-      <c r="E20" s="1">
+      <c r="F20" s="1">
         <v>6.66</v>
       </c>
-      <c r="F20" s="1">
+      <c r="G20" s="1">
         <v>122.6</v>
       </c>
-      <c r="G20" s="6">
+      <c r="H20" s="6">
         <v>37.5</v>
       </c>
-      <c r="H20" s="5">
+      <c r="I20" s="5">
         <v>87</v>
       </c>
-      <c r="I20" s="6">
+      <c r="J20" s="6">
         <v>14.7</v>
       </c>
-      <c r="J20" s="6">
+      <c r="K20" s="6">
         <v>157.19999999999999</v>
       </c>
-      <c r="K20" s="8">
+      <c r="L20" s="8">
         <v>6.14</v>
       </c>
-      <c r="L20" s="1" t="s">
+      <c r="M20" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="M20" s="1"/>
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
@@ -1882,8 +1944,9 @@
       <c r="AD20" s="1"/>
       <c r="AE20" s="1"/>
       <c r="AF20" s="1"/>
-    </row>
-    <row r="21" spans="1:32" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AG20" s="1"/>
+    </row>
+    <row r="21" spans="1:33" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="22" t="s">
         <v>43</v>
       </c>
@@ -1891,36 +1954,38 @@
         <v>36</v>
       </c>
       <c r="C21" s="8">
+        <v>42.46</v>
+      </c>
+      <c r="D21" s="8">
         <v>50</v>
       </c>
-      <c r="D21" s="6">
+      <c r="E21" s="6">
         <v>93.7</v>
       </c>
-      <c r="E21" s="1">
+      <c r="F21" s="1">
         <v>5.42</v>
       </c>
-      <c r="F21" s="1">
+      <c r="G21" s="1">
         <v>166.5</v>
       </c>
-      <c r="G21" s="6">
+      <c r="H21" s="6">
         <v>28</v>
       </c>
-      <c r="H21" s="5">
+      <c r="I21" s="5">
         <v>82</v>
       </c>
-      <c r="I21" s="6">
+      <c r="J21" s="6">
         <v>15.1</v>
       </c>
-      <c r="J21" s="6">
+      <c r="K21" s="6">
         <v>185.6</v>
       </c>
-      <c r="K21" s="8">
+      <c r="L21" s="8">
         <v>3.84</v>
       </c>
-      <c r="L21" s="1" t="s">
+      <c r="M21" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="M21" s="1"/>
       <c r="N21" s="1"/>
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
@@ -1940,8 +2005,9 @@
       <c r="AD21" s="1"/>
       <c r="AE21" s="1"/>
       <c r="AF21" s="1"/>
-    </row>
-    <row r="22" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AG21" s="1"/>
+    </row>
+    <row r="22" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="10" t="s">
         <v>11</v>
       </c>
@@ -1949,36 +2015,38 @@
         <v>93</v>
       </c>
       <c r="C22" s="8">
+        <v>97.1</v>
+      </c>
+      <c r="D22" s="8">
         <v>41</v>
       </c>
-      <c r="D22" s="1">
+      <c r="E22" s="1">
         <v>115.2</v>
       </c>
-      <c r="E22" s="1">
+      <c r="F22" s="1">
         <v>4.91</v>
       </c>
-      <c r="F22" s="1">
+      <c r="G22" s="1">
         <v>189.7</v>
       </c>
-      <c r="G22" s="1">
+      <c r="H22" s="1">
         <v>21.6</v>
       </c>
-      <c r="H22" s="1">
+      <c r="I22" s="1">
         <v>90</v>
       </c>
-      <c r="I22" s="1">
+      <c r="J22" s="1">
         <v>13.9</v>
       </c>
-      <c r="J22" s="1">
+      <c r="K22" s="1">
         <v>167.4</v>
       </c>
-      <c r="K22" s="1">
+      <c r="L22" s="1">
         <v>5.13</v>
       </c>
-      <c r="L22" s="1" t="s">
+      <c r="M22" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="M22" s="1"/>
       <c r="N22" s="1"/>
       <c r="O22" s="1"/>
       <c r="P22" s="1"/>
@@ -1990,15 +2058,16 @@
       <c r="V22" s="1"/>
       <c r="W22" s="1"/>
       <c r="X22" s="1"/>
-      <c r="Z22" s="1"/>
+      <c r="Y22" s="1"/>
       <c r="AA22" s="1"/>
       <c r="AB22" s="1"/>
       <c r="AC22" s="1"/>
       <c r="AD22" s="1"/>
       <c r="AE22" s="1"/>
       <c r="AF22" s="1"/>
-    </row>
-    <row r="23" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AG22" s="1"/>
+    </row>
+    <row r="23" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="10" t="s">
         <v>12</v>
       </c>
@@ -2006,36 +2075,38 @@
         <v>64</v>
       </c>
       <c r="C23" s="8">
+        <v>68.62</v>
+      </c>
+      <c r="D23" s="8">
         <v>34.4</v>
       </c>
-      <c r="D23" s="1">
+      <c r="E23" s="1">
         <v>75.5</v>
       </c>
-      <c r="E23" s="1">
+      <c r="F23" s="1">
         <v>4.3</v>
       </c>
-      <c r="F23" s="1">
+      <c r="G23" s="1">
         <v>166.2</v>
       </c>
-      <c r="G23" s="1">
+      <c r="H23" s="1">
         <v>20.2</v>
       </c>
-      <c r="H23" s="1">
+      <c r="I23" s="1">
         <v>88</v>
       </c>
-      <c r="I23" s="1">
+      <c r="J23" s="1">
         <v>14.3</v>
       </c>
-      <c r="J23" s="1">
+      <c r="K23" s="1">
         <v>130.9</v>
       </c>
-      <c r="K23" s="1">
+      <c r="L23" s="1">
         <v>5.44</v>
       </c>
-      <c r="L23" s="1" t="s">
+      <c r="M23" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="M23" s="1"/>
       <c r="N23" s="1"/>
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
@@ -2047,15 +2118,16 @@
       <c r="V23" s="1"/>
       <c r="W23" s="1"/>
       <c r="X23" s="1"/>
-      <c r="Z23" s="1"/>
+      <c r="Y23" s="1"/>
       <c r="AA23" s="1"/>
       <c r="AB23" s="1"/>
       <c r="AC23" s="1"/>
       <c r="AD23" s="1"/>
       <c r="AE23" s="1"/>
       <c r="AF23" s="1"/>
-    </row>
-    <row r="24" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AG23" s="1"/>
+    </row>
+    <row r="24" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="11" t="s">
         <v>13</v>
       </c>
@@ -2063,36 +2135,38 @@
         <v>94</v>
       </c>
       <c r="C24" s="8">
+        <v>88.62</v>
+      </c>
+      <c r="D24" s="8">
         <v>36.5</v>
       </c>
-      <c r="D24" s="1">
+      <c r="E24" s="1">
         <v>43.4</v>
       </c>
-      <c r="E24" s="1">
+      <c r="F24" s="1">
         <v>4.84</v>
       </c>
-      <c r="F24" s="1">
+      <c r="G24" s="1">
         <v>179.7</v>
       </c>
-      <c r="G24" s="1">
+      <c r="H24" s="1">
         <v>31</v>
       </c>
-      <c r="H24" s="1">
+      <c r="I24" s="1">
         <v>93</v>
       </c>
-      <c r="I24" s="1">
+      <c r="J24" s="1">
         <v>13.3</v>
       </c>
-      <c r="J24" s="1">
+      <c r="K24" s="1">
         <v>115.4</v>
       </c>
-      <c r="K24" s="1">
+      <c r="L24" s="1">
         <v>5.7</v>
       </c>
-      <c r="L24" s="1" t="s">
+      <c r="M24" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="M24" s="1"/>
       <c r="N24" s="1"/>
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
@@ -2104,15 +2178,16 @@
       <c r="V24" s="1"/>
       <c r="W24" s="1"/>
       <c r="X24" s="1"/>
-      <c r="Z24" s="1"/>
+      <c r="Y24" s="1"/>
       <c r="AA24" s="1"/>
       <c r="AB24" s="1"/>
       <c r="AC24" s="1"/>
       <c r="AD24" s="1"/>
       <c r="AE24" s="1"/>
       <c r="AF24" s="1"/>
-    </row>
-    <row r="25" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AG24" s="1"/>
+    </row>
+    <row r="25" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="11" t="s">
         <v>14</v>
       </c>
@@ -2120,36 +2195,38 @@
         <v>66</v>
       </c>
       <c r="C25" s="8">
+        <v>69.790000000000006</v>
+      </c>
+      <c r="D25" s="8">
         <v>35.1</v>
       </c>
-      <c r="D25" s="1">
+      <c r="E25" s="1">
         <v>71.8</v>
       </c>
-      <c r="E25" s="1">
+      <c r="F25" s="1">
         <v>5.88</v>
       </c>
-      <c r="F25" s="1">
+      <c r="G25" s="1">
         <v>147.6</v>
       </c>
-      <c r="G25" s="1">
+      <c r="H25" s="1">
         <v>28.2</v>
       </c>
-      <c r="H25" s="1">
+      <c r="I25" s="1">
         <v>94</v>
       </c>
-      <c r="I25" s="1">
+      <c r="J25" s="1">
         <v>12.9</v>
       </c>
-      <c r="J25" s="1">
+      <c r="K25" s="1">
         <v>103.1</v>
       </c>
-      <c r="K25" s="1">
+      <c r="L25" s="1">
         <v>8.17</v>
       </c>
-      <c r="L25" s="1" t="s">
+      <c r="M25" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="M25" s="1"/>
       <c r="N25" s="1"/>
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
@@ -2161,15 +2238,16 @@
       <c r="V25" s="1"/>
       <c r="W25" s="1"/>
       <c r="X25" s="1"/>
-      <c r="Z25" s="1"/>
+      <c r="Y25" s="1"/>
       <c r="AA25" s="1"/>
       <c r="AB25" s="1"/>
       <c r="AC25" s="1"/>
       <c r="AD25" s="1"/>
       <c r="AE25" s="1"/>
       <c r="AF25" s="1"/>
-    </row>
-    <row r="26" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AG25" s="1"/>
+    </row>
+    <row r="26" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="12" t="s">
         <v>15</v>
       </c>
@@ -2177,36 +2255,38 @@
         <v>91</v>
       </c>
       <c r="C26" s="8">
+        <v>99.53</v>
+      </c>
+      <c r="D26" s="8">
         <v>27.8</v>
       </c>
-      <c r="D26" s="1">
+      <c r="E26" s="1">
         <v>62.7</v>
       </c>
-      <c r="E26" s="1">
+      <c r="F26" s="1">
         <v>4.1399999999999997</v>
       </c>
-      <c r="F26" s="1">
+      <c r="G26" s="1">
         <v>140.9</v>
       </c>
-      <c r="G26" s="1">
+      <c r="H26" s="1">
         <v>26.3</v>
       </c>
-      <c r="H26" s="1">
+      <c r="I26" s="1">
         <v>64</v>
       </c>
-      <c r="I26" s="1">
+      <c r="J26" s="1">
         <v>16.7</v>
       </c>
-      <c r="J26" s="1">
+      <c r="K26" s="1">
         <v>173.5</v>
       </c>
-      <c r="K26" s="1">
+      <c r="L26" s="1">
         <v>12.6</v>
       </c>
-      <c r="L26" s="1" t="s">
+      <c r="M26" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="M26" s="1"/>
       <c r="N26" s="1"/>
       <c r="O26" s="1"/>
       <c r="P26" s="1"/>
@@ -2226,8 +2306,9 @@
       <c r="AD26" s="1"/>
       <c r="AE26" s="1"/>
       <c r="AF26" s="1"/>
-    </row>
-    <row r="27" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AG26" s="1"/>
+    </row>
+    <row r="27" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="12" t="s">
         <v>16</v>
       </c>
@@ -2235,36 +2316,38 @@
         <v>69</v>
       </c>
       <c r="C27" s="8">
+        <v>73.59</v>
+      </c>
+      <c r="D27" s="8">
         <v>26</v>
       </c>
-      <c r="D27" s="1">
+      <c r="E27" s="1">
         <v>60.5</v>
       </c>
-      <c r="E27" s="1">
+      <c r="F27" s="1">
         <v>4.38</v>
       </c>
-      <c r="F27" s="1">
+      <c r="G27" s="1">
         <v>141.9</v>
       </c>
-      <c r="G27" s="1">
+      <c r="H27" s="1">
         <v>44.8</v>
       </c>
-      <c r="H27" s="1">
+      <c r="I27" s="1">
         <v>79</v>
       </c>
-      <c r="I27" s="1">
+      <c r="J27" s="1">
         <v>15.1</v>
       </c>
-      <c r="J27" s="1">
+      <c r="K27" s="1">
         <v>203.8</v>
       </c>
-      <c r="K27" s="1">
+      <c r="L27" s="1">
         <v>6</v>
       </c>
-      <c r="L27" s="1" t="s">
+      <c r="M27" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="M27" s="1"/>
       <c r="N27" s="1"/>
       <c r="O27" s="1"/>
       <c r="P27" s="1"/>
@@ -2284,45 +2367,48 @@
       <c r="AD27" s="1"/>
       <c r="AE27" s="1"/>
       <c r="AF27" s="1"/>
-    </row>
-    <row r="28" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AG27" s="1"/>
+    </row>
+    <row r="28" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="13" t="s">
         <v>17</v>
       </c>
       <c r="B28" s="9">
         <v>0</v>
       </c>
-      <c r="C28" s="8">
+      <c r="C28" s="9">
+        <v>14.8</v>
+      </c>
+      <c r="D28" s="8">
         <v>69.099999999999994</v>
       </c>
-      <c r="D28" s="1">
+      <c r="E28" s="1">
         <v>67</v>
       </c>
-      <c r="E28" s="1">
+      <c r="F28" s="1">
         <v>3.22</v>
       </c>
-      <c r="F28" s="1">
+      <c r="G28" s="1">
         <v>264.8</v>
       </c>
-      <c r="G28" s="1">
+      <c r="H28" s="1">
         <v>40.299999999999997</v>
       </c>
-      <c r="H28" s="1">
+      <c r="I28" s="1">
         <v>112</v>
       </c>
-      <c r="I28" s="1">
+      <c r="J28" s="1">
         <v>16.8</v>
       </c>
-      <c r="J28" s="1">
+      <c r="K28" s="1">
         <v>264</v>
       </c>
-      <c r="K28" s="3">
+      <c r="L28" s="3">
         <v>9.9499999999999993</v>
       </c>
-      <c r="L28" s="1" t="s">
+      <c r="M28" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="M28" s="1"/>
       <c r="N28" s="1"/>
       <c r="O28" s="1"/>
       <c r="P28" s="1"/>
@@ -2342,8 +2428,9 @@
       <c r="AD28" s="1"/>
       <c r="AE28" s="1"/>
       <c r="AF28" s="1"/>
-    </row>
-    <row r="29" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AG28" s="1"/>
+    </row>
+    <row r="29" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="14" t="s">
         <v>18</v>
       </c>
@@ -2351,37 +2438,40 @@
         <v>86</v>
       </c>
       <c r="C29" s="9">
+        <v>89.42</v>
+      </c>
+      <c r="D29" s="9">
         <v>35.1</v>
       </c>
-      <c r="D29" s="3">
+      <c r="E29" s="3">
         <v>69.099999999999994</v>
       </c>
-      <c r="E29" s="3">
+      <c r="F29" s="3">
         <v>4.95</v>
       </c>
-      <c r="F29" s="3">
+      <c r="G29" s="3">
         <v>138.80000000000001</v>
       </c>
-      <c r="G29" s="3">
+      <c r="H29" s="3">
         <v>20.6</v>
       </c>
-      <c r="H29" s="3">
+      <c r="I29" s="3">
         <v>109</v>
       </c>
-      <c r="I29" s="3">
+      <c r="J29" s="3">
         <v>12.5</v>
       </c>
-      <c r="J29" s="3">
+      <c r="K29" s="3">
         <v>135.19999999999999</v>
       </c>
-      <c r="K29" s="3">
+      <c r="L29" s="3">
         <v>7.26</v>
       </c>
-      <c r="L29" s="3" t="s">
+      <c r="M29" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="30" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="14" t="s">
         <v>19</v>
       </c>
@@ -2389,37 +2479,40 @@
         <v>32</v>
       </c>
       <c r="C30" s="9">
+        <v>21.09</v>
+      </c>
+      <c r="D30" s="9">
         <v>61.3</v>
       </c>
-      <c r="D30" s="3">
+      <c r="E30" s="3">
         <v>39.4</v>
       </c>
-      <c r="E30" s="3">
+      <c r="F30" s="3">
         <v>3.74</v>
       </c>
-      <c r="F30" s="3">
+      <c r="G30" s="3">
         <v>107</v>
       </c>
-      <c r="G30" s="3">
+      <c r="H30" s="3">
         <v>21.1</v>
       </c>
-      <c r="H30" s="3">
+      <c r="I30" s="3">
         <v>101</v>
       </c>
-      <c r="I30" s="3">
+      <c r="J30" s="3">
         <v>12.1</v>
       </c>
-      <c r="J30" s="3">
+      <c r="K30" s="3">
         <v>151</v>
       </c>
-      <c r="K30" s="3">
+      <c r="L30" s="3">
         <v>5.68</v>
       </c>
-      <c r="L30" s="3" t="s">
+      <c r="M30" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="31" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="15" t="s">
         <v>20</v>
       </c>
@@ -2427,37 +2520,40 @@
         <v>94</v>
       </c>
       <c r="C31" s="9">
+        <v>96.25</v>
+      </c>
+      <c r="D31" s="9">
         <v>45.6</v>
       </c>
-      <c r="D31" s="3">
+      <c r="E31" s="3">
         <v>51.7</v>
       </c>
-      <c r="E31" s="3">
+      <c r="F31" s="3">
         <v>5.3</v>
       </c>
-      <c r="F31" s="3">
+      <c r="G31" s="3">
         <v>120</v>
       </c>
-      <c r="G31" s="3">
+      <c r="H31" s="3">
         <v>26.3</v>
       </c>
-      <c r="H31" s="3">
+      <c r="I31" s="3">
         <v>112</v>
       </c>
-      <c r="I31" s="3">
+      <c r="J31" s="3">
         <v>13.5</v>
       </c>
-      <c r="J31" s="3">
+      <c r="K31" s="3">
         <v>210</v>
       </c>
-      <c r="K31" s="3">
+      <c r="L31" s="3">
         <v>6.24</v>
       </c>
-      <c r="L31" s="3" t="s">
+      <c r="M31" s="3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="32" spans="1:32" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:33" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="23" t="s">
         <v>21</v>
       </c>
@@ -2465,37 +2561,40 @@
         <v>0</v>
       </c>
       <c r="C32" s="24">
+        <v>24.83</v>
+      </c>
+      <c r="D32" s="24">
         <v>48.1</v>
       </c>
-      <c r="D32" s="25">
+      <c r="E32" s="25">
         <v>46.1</v>
       </c>
-      <c r="E32" s="25">
+      <c r="F32" s="25">
         <v>7.24</v>
       </c>
-      <c r="F32" s="25">
+      <c r="G32" s="25">
         <v>67.2</v>
       </c>
-      <c r="G32" s="25">
+      <c r="H32" s="25">
         <v>12.9</v>
       </c>
-      <c r="H32" s="25">
+      <c r="I32" s="25">
         <v>109</v>
       </c>
-      <c r="I32" s="25">
+      <c r="J32" s="25">
         <v>15.8</v>
       </c>
-      <c r="J32" s="25">
+      <c r="K32" s="25">
         <v>246</v>
       </c>
-      <c r="K32" s="25">
+      <c r="L32" s="25">
         <v>6.08</v>
       </c>
-      <c r="L32" s="25" t="s">
+      <c r="M32" s="25" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="16" t="s">
         <v>22</v>
       </c>
@@ -2503,37 +2602,40 @@
         <v>91</v>
       </c>
       <c r="C33" s="9">
+        <v>112.98</v>
+      </c>
+      <c r="D33" s="9">
         <v>36.6</v>
       </c>
-      <c r="D33" s="3">
+      <c r="E33" s="3">
         <v>62.9</v>
       </c>
-      <c r="E33" s="3">
+      <c r="F33" s="3">
         <v>5.33</v>
       </c>
-      <c r="F33" s="3">
+      <c r="G33" s="3">
         <v>214</v>
       </c>
-      <c r="G33" s="3">
+      <c r="H33" s="3">
         <v>16.600000000000001</v>
       </c>
-      <c r="H33" s="3">
+      <c r="I33" s="3">
         <v>106</v>
       </c>
-      <c r="I33" s="3">
+      <c r="J33" s="3">
         <v>16.899999999999999</v>
       </c>
-      <c r="J33" s="3">
+      <c r="K33" s="3">
         <v>324</v>
       </c>
-      <c r="K33" s="3">
+      <c r="L33" s="3">
         <v>6.51</v>
       </c>
-      <c r="L33" s="3" t="s">
+      <c r="M33" s="3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="34" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="16" t="s">
         <v>23</v>
       </c>
@@ -2541,37 +2643,40 @@
         <v>65</v>
       </c>
       <c r="C34" s="9">
+        <v>86.27</v>
+      </c>
+      <c r="D34" s="9">
         <v>18.7</v>
       </c>
-      <c r="D34" s="3">
+      <c r="E34" s="3">
         <v>80.5</v>
       </c>
-      <c r="E34" s="3">
+      <c r="F34" s="3">
         <v>8.35</v>
       </c>
-      <c r="F34" s="3">
+      <c r="G34" s="3">
         <v>137.9</v>
       </c>
-      <c r="G34" s="3">
+      <c r="H34" s="3">
         <v>39.4</v>
       </c>
-      <c r="H34" s="3">
+      <c r="I34" s="3">
         <v>106</v>
       </c>
-      <c r="I34" s="3">
+      <c r="J34" s="3">
         <v>12.7</v>
       </c>
-      <c r="J34" s="3">
+      <c r="K34" s="3">
         <v>181</v>
       </c>
-      <c r="K34" s="3">
+      <c r="L34" s="3">
         <v>11.49</v>
       </c>
-      <c r="L34" s="3" t="s">
+      <c r="M34" s="3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="35" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="19" t="s">
         <v>44</v>
       </c>
@@ -2579,37 +2684,40 @@
         <v>94</v>
       </c>
       <c r="C35" s="9">
+        <v>102.64</v>
+      </c>
+      <c r="D35" s="9">
         <v>43.7</v>
       </c>
-      <c r="D35" s="3">
+      <c r="E35" s="3">
         <v>51.6</v>
       </c>
-      <c r="E35" s="3">
+      <c r="F35" s="3">
         <v>6.19</v>
       </c>
-      <c r="F35" s="3">
+      <c r="G35" s="3">
         <v>121.8</v>
       </c>
-      <c r="G35" s="3">
+      <c r="H35" s="3">
         <v>33.200000000000003</v>
       </c>
-      <c r="H35" s="3">
+      <c r="I35" s="3">
         <v>102</v>
       </c>
-      <c r="I35" s="3">
+      <c r="J35" s="3">
         <v>15.7</v>
       </c>
-      <c r="J35" s="3">
+      <c r="K35" s="3">
         <v>179</v>
       </c>
-      <c r="K35" s="3">
+      <c r="L35" s="3">
         <v>6.62</v>
       </c>
-      <c r="L35" s="3" t="s">
+      <c r="M35" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="19" t="s">
         <v>45</v>
       </c>
@@ -2617,37 +2725,40 @@
         <v>66</v>
       </c>
       <c r="C36" s="9">
+        <v>70.290000000000006</v>
+      </c>
+      <c r="D36" s="9">
         <v>40.4</v>
       </c>
-      <c r="D36" s="3">
+      <c r="E36" s="3">
         <v>35.6</v>
       </c>
-      <c r="E36" s="3">
+      <c r="F36" s="3">
         <v>5.98</v>
       </c>
-      <c r="F36" s="3">
+      <c r="G36" s="3">
         <v>110.7</v>
       </c>
-      <c r="G36" s="3">
+      <c r="H36" s="3">
         <v>18.100000000000001</v>
       </c>
-      <c r="H36" s="3">
+      <c r="I36" s="3">
         <v>115</v>
       </c>
-      <c r="I36" s="3">
+      <c r="J36" s="3">
         <v>13.2</v>
       </c>
-      <c r="J36" s="3">
+      <c r="K36" s="3">
         <v>153</v>
       </c>
-      <c r="K36" s="3">
+      <c r="L36" s="3">
         <v>2.42</v>
       </c>
-      <c r="L36" s="3" t="s">
+      <c r="M36" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="37" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="19" t="s">
         <v>46</v>
       </c>
@@ -2655,37 +2766,40 @@
         <v>35</v>
       </c>
       <c r="C37" s="9">
+        <v>38.31</v>
+      </c>
+      <c r="D37" s="9">
         <v>41.5</v>
       </c>
-      <c r="D37" s="3">
+      <c r="E37" s="3">
         <v>37.200000000000003</v>
       </c>
-      <c r="E37" s="3">
+      <c r="F37" s="3">
         <v>6.33</v>
       </c>
-      <c r="F37" s="3">
+      <c r="G37" s="3">
         <v>90.7</v>
       </c>
-      <c r="G37" s="3">
+      <c r="H37" s="3">
         <v>40</v>
       </c>
-      <c r="H37" s="3">
+      <c r="I37" s="3">
         <v>111</v>
       </c>
-      <c r="I37" s="3">
+      <c r="J37" s="3">
         <v>13</v>
       </c>
-      <c r="J37" s="3">
+      <c r="K37" s="3">
         <v>86.9</v>
       </c>
-      <c r="K37" s="3">
+      <c r="L37" s="3">
         <v>4.8</v>
       </c>
-      <c r="L37" s="3" t="s">
+      <c r="M37" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="38" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="19" t="s">
         <v>47</v>
       </c>
@@ -2693,55 +2807,58 @@
         <v>84</v>
       </c>
       <c r="C38" s="9">
+        <v>85.65</v>
+      </c>
+      <c r="D38" s="9">
         <v>51.9</v>
       </c>
-      <c r="D38" s="3">
+      <c r="E38" s="3">
         <v>50.8</v>
       </c>
-      <c r="E38" s="3">
+      <c r="F38" s="3">
         <v>6.87</v>
       </c>
-      <c r="F38" s="3">
+      <c r="G38" s="3">
         <v>141.19999999999999</v>
       </c>
-      <c r="G38" s="3">
+      <c r="H38" s="3">
         <v>37.700000000000003</v>
       </c>
-      <c r="H38" s="3">
+      <c r="I38" s="3">
         <v>107</v>
       </c>
-      <c r="I38" s="3">
+      <c r="J38" s="3">
         <v>13.6</v>
       </c>
-      <c r="J38" s="3">
+      <c r="K38" s="3">
         <v>232.9</v>
       </c>
-      <c r="K38" s="3">
+      <c r="L38" s="3">
         <v>5.32</v>
       </c>
-      <c r="L38" s="3" t="s">
+      <c r="M38" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="39" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="17"/>
     </row>
-    <row r="40" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="17"/>
     </row>
-    <row r="41" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="17"/>
     </row>
-    <row r="42" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="17"/>
     </row>
-    <row r="43" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="17"/>
     </row>
-    <row r="44" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="17"/>
     </row>
-    <row r="45" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="17"/>
     </row>
   </sheetData>

</xml_diff>